<commit_message>
Fix of switching to start position
</commit_message>
<xml_diff>
--- a/Регистры_управления_драйвером.xlsx
+++ b/Регистры_управления_драйвером.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
   <si>
     <t>Read/Write</t>
   </si>
@@ -138,6 +138,12 @@
   </si>
   <si>
     <t>6414-65534</t>
+  </si>
+  <si>
+    <t>Состояние дискретных входов</t>
+  </si>
+  <si>
+    <t>Текущее положение заслонки</t>
   </si>
 </sst>
 </file>
@@ -211,17 +217,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -570,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5:E32"/>
+  <dimension ref="A5:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,7 +788,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C29" s="3"/>
+      <c r="C29" s="2"/>
       <c r="D29" s="1" t="s">
         <v>32</v>
       </c>
@@ -788,27 +797,49 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C30" s="4"/>
+      <c r="C30" s="3"/>
       <c r="D30" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E30" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C31" s="4"/>
+      <c r="C31" s="3"/>
       <c r="D31" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E31" s="2"/>
+      <c r="E31" s="5"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C32" s="5"/>
+      <c r="C32" s="4"/>
       <c r="D32" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E32" s="2"/>
+      <c r="E32" s="5"/>
+    </row>
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34">
+        <v>30005</v>
+      </c>
+      <c r="C34" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35">
+        <v>30006</v>
+      </c>
+      <c r="C35" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>